<commit_message>
Created new suite xml file for new pages
</commit_message>
<xml_diff>
--- a/LearnSmartAutomation/TestCaseData1.xlsx
+++ b/LearnSmartAutomation/TestCaseData1.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\LearnSmartAutomation\LearnSmartAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE400E25-BCEF-4A8C-AD5B-6358D843F081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7361587A-94FD-48C1-9A8B-C0B220B331FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DemoTestCaseSheet" sheetId="1" r:id="rId1"/>
     <sheet name="SectionTestSuite" sheetId="2" r:id="rId2"/>
+    <sheet name="LessonsTestSuite" sheetId="3" r:id="rId3"/>
+    <sheet name="TopicsTestSuite" sheetId="4" r:id="rId4"/>
+    <sheet name="ContentsTestSuite" sheetId="5" r:id="rId5"/>
+    <sheet name="QuizzesTestSuite" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DemoTestCaseSheet!$A$1:$P$1</definedName>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="76">
   <si>
     <t>Sr.No</t>
   </si>
@@ -131,9 +135,6 @@
     <t>Edited Course</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>lessonsFlag</t>
   </si>
   <si>
@@ -153,6 +154,108 @@
   </si>
   <si>
     <t>section001</t>
+  </si>
+  <si>
+    <t>Lessons</t>
+  </si>
+  <si>
+    <t>topicsFlag</t>
+  </si>
+  <si>
+    <t>topicsName</t>
+  </si>
+  <si>
+    <t>lessionName</t>
+  </si>
+  <si>
+    <t>Sample Topic 54</t>
+  </si>
+  <si>
+    <t>Topics</t>
+  </si>
+  <si>
+    <t>topicName</t>
+  </si>
+  <si>
+    <t>contentsFlag</t>
+  </si>
+  <si>
+    <t>contentsName</t>
+  </si>
+  <si>
+    <t>JEE mains section 1 lesson 2 topic 2 content 2</t>
+  </si>
+  <si>
+    <t>topics001</t>
+  </si>
+  <si>
+    <t>Topics Description</t>
+  </si>
+  <si>
+    <t>contentType</t>
+  </si>
+  <si>
+    <t>contentName</t>
+  </si>
+  <si>
+    <t>Contents_1</t>
+  </si>
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>contentsDetails</t>
+  </si>
+  <si>
+    <t>Enter contents detils</t>
+  </si>
+  <si>
+    <t>Contents</t>
+  </si>
+  <si>
+    <t>Quizzes</t>
+  </si>
+  <si>
+    <t>quizType</t>
+  </si>
+  <si>
+    <t>quizName</t>
+  </si>
+  <si>
+    <t>durationInMin</t>
+  </si>
+  <si>
+    <t>passingPercn</t>
+  </si>
+  <si>
+    <t>autoSubmitFlag</t>
+  </si>
+  <si>
+    <t>MCQ</t>
+  </si>
+  <si>
+    <t>quizzes_1</t>
+  </si>
+  <si>
+    <t>Quizzes Auto</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>quizPrice</t>
+  </si>
+  <si>
+    <t>questionsTabFlag</t>
+  </si>
+  <si>
+    <t>questionsBankName</t>
+  </si>
+  <si>
+    <t>Direct Tax Test 1</t>
+  </si>
+  <si>
+    <t>Psychometric Test</t>
   </si>
 </sst>
 </file>
@@ -187,7 +290,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,6 +300,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -228,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -239,13 +348,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,9 +658,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,7 +801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="28.8" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -697,8 +832,8 @@
       <c r="K3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>35</v>
+      <c r="L3" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>33</v>
@@ -727,21 +862,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BE89DB3-C9A9-4857-B9A2-8385FA47631F}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="4"/>
-    <col min="6" max="6" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="13" width="8.88671875" style="4"/>
-    <col min="14" max="14" width="10" style="4" customWidth="1"/>
-    <col min="15" max="15" width="10.21875" style="4" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="5.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="6"/>
+    <col min="6" max="6" width="8.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="8.88671875" style="6"/>
+    <col min="12" max="12" width="8.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="6"/>
+    <col min="14" max="14" width="10" style="6" customWidth="1"/>
+    <col min="15" max="15" width="10.21875" style="6" customWidth="1"/>
+    <col min="16" max="16" width="8.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -782,61 +920,588 @@
         <v>15</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4">
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6">
+        <v>1</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="6">
+        <v>1</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="6">
+        <v>1</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000106FD-F9BD-4289-AC1F-6B239EC41A22}">
+  <dimension ref="A1:Q4"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="9"/>
+    <col min="2" max="2" width="22.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="9"/>
+    <col min="8" max="8" width="16.88671875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="9"/>
+    <col min="10" max="10" width="10.33203125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" style="9" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" style="9" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="9"/>
+    <col min="14" max="14" width="12.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="9"/>
+    <col min="16" max="16" width="21.5546875" style="9" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10">
+        <v>1</v>
+      </c>
+      <c r="E2" s="10">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="10">
+        <v>1</v>
+      </c>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10">
+        <v>1</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="10">
+        <v>1</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" s="10">
+        <v>1</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" s="10"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N3" s="18"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N4" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1FD572-205B-4877-A5E2-B94191D576F1}">
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="7" width="8.88671875" style="10"/>
+    <col min="8" max="8" width="13.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.88671875" style="10"/>
+    <col min="11" max="11" width="13.21875" style="10" customWidth="1"/>
+    <col min="12" max="12" width="10.21875" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="10"/>
+    <col min="14" max="14" width="37.21875" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="10"/>
+    <col min="16" max="16" width="18.44140625" style="10" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="28.8" x14ac:dyDescent="0.2">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="10">
+        <v>1</v>
+      </c>
+      <c r="E2" s="10">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="10">
+        <v>1</v>
+      </c>
+      <c r="J2" s="10">
+        <v>1</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="10">
+        <v>1</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" s="10">
+        <v>1</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C612BDD1-2840-4200-8344-FE92A8CAB7A2}">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="11" max="11" width="13.88671875" customWidth="1"/>
+    <col min="12" max="13" width="19.88671875" customWidth="1"/>
+    <col min="14" max="14" width="8.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+    </row>
+    <row r="2" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
         <v>1</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" s="4">
-        <v>1</v>
-      </c>
-      <c r="J2" s="4">
-        <v>1</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" s="4" t="s">
+      <c r="G2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB833CE-4F77-45DD-8602-43A23E9E2294}">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="15" width="8.88671875" style="9"/>
+    <col min="16" max="16" width="7.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" style="9"/>
+    <col min="18" max="18" width="16.5546875" style="9" customWidth="1"/>
+    <col min="19" max="19" width="15.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="4">
-        <v>1</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="O1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" s="2">
+        <v>10</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O2" s="9">
+        <v>50</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2" s="9">
+        <v>200</v>
+      </c>
+      <c r="R2" s="14">
+        <v>1</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="T2" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added New Module Admin
</commit_message>
<xml_diff>
--- a/LearnSmartAutomation/TestCaseData1.xlsx
+++ b/LearnSmartAutomation/TestCaseData1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\LearnSmartAutomation\LearnSmartAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7361587A-94FD-48C1-9A8B-C0B220B331FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722E8A25-49FB-4EC0-8A00-DABAB3975A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DemoTestCaseSheet" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="TopicsTestSuite" sheetId="4" r:id="rId4"/>
     <sheet name="ContentsTestSuite" sheetId="5" r:id="rId5"/>
     <sheet name="QuizzesTestSuite" sheetId="6" r:id="rId6"/>
+    <sheet name="QuestionsTestSuite" sheetId="7" r:id="rId7"/>
+    <sheet name="AdminModule" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DemoTestCaseSheet!$A$1:$P$1</definedName>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="98">
   <si>
     <t>Sr.No</t>
   </si>
@@ -256,13 +258,79 @@
   </si>
   <si>
     <t>Psychometric Test</t>
+  </si>
+  <si>
+    <t>sequence</t>
+  </si>
+  <si>
+    <t>marks</t>
+  </si>
+  <si>
+    <t>module</t>
+  </si>
+  <si>
+    <t>subModule</t>
+  </si>
+  <si>
+    <t>questionName</t>
+  </si>
+  <si>
+    <t>difficultyLevel</t>
+  </si>
+  <si>
+    <t>questionText</t>
+  </si>
+  <si>
+    <t>ques1</t>
+  </si>
+  <si>
+    <t>Question Auto</t>
+  </si>
+  <si>
+    <t>questionsType</t>
+  </si>
+  <si>
+    <t>Subjective - Textbox</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>newUserFlag</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>autoTest@q.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,6 +357,28 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF202124"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -310,7 +400,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -333,11 +423,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -371,18 +473,42 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -658,9 +784,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P6" sqref="P6"/>
+      <selection pane="topRight" activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1103,7 +1229,7 @@
       <c r="M2" s="10">
         <v>1</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="14" t="s">
         <v>46</v>
       </c>
       <c r="O2" s="10">
@@ -1115,10 +1241,10 @@
       <c r="Q2" s="10"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="N3" s="18"/>
+      <c r="N3" s="15"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="N4" s="18"/>
+      <c r="N4" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1370,23 +1496,25 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB833CE-4F77-45DD-8602-43A23E9E2294}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="15" width="8.88671875" style="9"/>
-    <col min="16" max="16" width="7.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.88671875" style="9"/>
-    <col min="18" max="18" width="16.5546875" style="9" customWidth="1"/>
-    <col min="19" max="19" width="15.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="15" width="8.88671875" style="17"/>
+    <col min="16" max="16" width="7.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" style="17"/>
+    <col min="18" max="18" width="16.5546875" style="17" customWidth="1"/>
+    <col min="19" max="19" width="15.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.88671875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1444,8 +1572,14 @@
       <c r="S1" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="T1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1464,7 +1598,7 @@
       <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="18" t="s">
         <v>61</v>
       </c>
       <c r="H2" s="2">
@@ -1486,25 +1620,231 @@
       <c r="N2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="O2" s="9">
+      <c r="O2" s="17">
         <v>50</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="Q2" s="9">
+      <c r="Q2" s="17">
         <v>200</v>
       </c>
-      <c r="R2" s="14">
-        <v>1</v>
-      </c>
-      <c r="S2" s="16" t="s">
+      <c r="R2" s="13">
+        <v>1</v>
+      </c>
+      <c r="S2" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="T2" s="15"/>
+      <c r="T2" s="16">
+        <v>1</v>
+      </c>
+      <c r="U2" s="17">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDC74F27-38F5-4B0C-B4F0-0243E583C7E0}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="6" width="8.88671875" style="21"/>
+    <col min="7" max="7" width="12.88671875" style="21" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="21"/>
+    <col min="9" max="9" width="8.33203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5546875" style="21" customWidth="1"/>
+    <col min="12" max="12" width="25" style="21" customWidth="1"/>
+    <col min="13" max="13" width="26" style="21" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="21">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="21">
+        <v>1</v>
+      </c>
+      <c r="E2" s="21">
+        <v>1</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="21">
+        <v>1</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="L2" s="22">
+        <v>3</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95DC6DAF-3E6E-4517-8A47-7DB48C80CEF1}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="L1" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="M1" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="21">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="21">
+        <v>1</v>
+      </c>
+      <c r="E2" s="21">
+        <v>1</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2" t="s">
+        <v>95</v>
+      </c>
+      <c r="K2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L2" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{24AEBD8C-9EFA-4E23-96F0-48D011BFE7C6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>